<commit_message>
lots of new plots
</commit_message>
<xml_diff>
--- a/Data/Acute-OA-Trial.xlsx
+++ b/Data/Acute-OA-Trial.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28331"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/roberts-lab/O.lurida_Stress/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11725D6-D27B-9E47-8EF6-73A88668B8B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="13300" windowHeight="15440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="26220" windowHeight="17220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tissue Samples" sheetId="1" r:id="rId1"/>
     <sheet name="Water chemistry" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="64">
   <si>
     <t>Sample #</t>
   </si>
@@ -207,14 +218,20 @@
   <si>
     <t>Standard</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Extracted 2/15/19 to test protocol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -500,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -730,6 +747,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1054,14 +1079,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H187"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I187"/>
   <sheetViews>
-    <sheetView topLeftCell="A173" workbookViewId="0">
-      <selection sqref="A1:D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1080" topLeftCell="A173" activePane="bottomLeft"/>
+      <selection activeCell="A19" sqref="A2:XFD19"/>
+      <selection pane="bottomLeft" activeCell="G185" sqref="G185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
@@ -1070,7 +1097,7 @@
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -1090,7 +1117,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1111,7 +1138,7 @@
         <v>14.155000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1132,7 +1159,7 @@
         <v>13.370000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1153,7 +1180,7 @@
         <v>13.645</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1174,7 +1201,7 @@
         <v>11.155000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +1222,7 @@
         <v>10.16</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1216,7 +1243,7 @@
         <v>15.425000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1237,7 +1264,7 @@
         <v>14.435</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1258,7 +1285,7 @@
         <v>15.32</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1279,7 +1306,7 @@
         <v>14.844999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1300,7 +1327,7 @@
         <v>14.81</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1321,7 +1348,7 @@
         <v>14.05</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1342,7 +1369,7 @@
         <v>15.059999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1363,7 +1390,7 @@
         <v>14.254999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1384,7 +1411,7 @@
         <v>17.84</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1405,7 +1432,7 @@
         <v>17.625</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1426,7 +1453,7 @@
         <v>15.32</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1447,7 +1474,8 @@
         <v>13.03</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1472,8 +1500,11 @@
       <c r="H20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1493,14 +1524,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G21" s="1">
-        <f>F21-$G$1</f>
+        <f t="shared" ref="G21:G52" si="0">F21-$G$1</f>
         <v>0.23958333333333337</v>
       </c>
       <c r="H21">
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1520,14 +1551,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G22" s="1">
-        <f>F22-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H22">
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1547,14 +1578,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G23" s="1">
-        <f>F23-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H23">
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1574,14 +1605,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G24" s="1">
-        <f>F24-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H24">
         <v>1.6</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1601,14 +1632,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G25" s="1">
-        <f>F25-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H25">
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1628,14 +1659,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G26" s="1">
-        <f>F26-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H26">
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1655,14 +1686,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G27" s="1">
-        <f>F27-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H27">
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
@@ -1682,14 +1713,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G28" s="1">
-        <f>F28-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H28">
         <v>1.6</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1709,14 +1740,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G29" s="1">
-        <f>F29-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H29">
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1736,14 +1767,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G30" s="1">
-        <f>F30-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H30">
         <v>1.6</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11</v>
       </c>
@@ -1763,14 +1794,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G31" s="1">
-        <f>F31-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H31">
         <v>1.6</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>12</v>
       </c>
@@ -1790,14 +1821,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G32" s="1">
-        <f>F32-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H32">
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>13</v>
       </c>
@@ -1817,14 +1848,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G33" s="1">
-        <f>F33-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H33">
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>14</v>
       </c>
@@ -1844,14 +1875,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G34" s="1">
-        <f>F34-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H34">
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>15</v>
       </c>
@@ -1871,14 +1902,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G35" s="1">
-        <f>F35-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H35">
         <v>1.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>16</v>
       </c>
@@ -1898,14 +1929,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G36" s="1">
-        <f>F36-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H36">
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>17</v>
       </c>
@@ -1925,14 +1956,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G37" s="1">
-        <f>F37-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H37">
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>18</v>
       </c>
@@ -1952,14 +1983,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G38" s="1">
-        <f>F38-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H38">
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>19</v>
       </c>
@@ -1979,14 +2010,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G39" s="1">
-        <f>F39-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H39">
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>20</v>
       </c>
@@ -2006,14 +2037,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G40" s="1">
-        <f>F40-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H40">
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>21</v>
       </c>
@@ -2033,14 +2064,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G41" s="1">
-        <f>F41-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H41">
         <v>1.6</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>22</v>
       </c>
@@ -2060,14 +2091,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G42" s="1">
-        <f>F42-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H42">
         <v>1.6</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>23</v>
       </c>
@@ -2087,14 +2118,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G43" s="1">
-        <f>F43-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H43">
         <v>1.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>24</v>
       </c>
@@ -2114,14 +2145,14 @@
         <v>0.76736111111111116</v>
       </c>
       <c r="G44" s="1">
-        <f>F44-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.23958333333333337</v>
       </c>
       <c r="H44">
         <v>1.5</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>25</v>
       </c>
@@ -2141,14 +2172,14 @@
         <v>0.78125</v>
       </c>
       <c r="G45" s="1">
-        <f>F45-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H45">
         <v>1.6</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>26</v>
       </c>
@@ -2168,14 +2199,14 @@
         <v>0.78125</v>
       </c>
       <c r="G46" s="1">
-        <f>F46-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H46">
         <v>1.6</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>27</v>
       </c>
@@ -2195,14 +2226,14 @@
         <v>0.78125</v>
       </c>
       <c r="G47" s="1">
-        <f>F47-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H47">
         <v>1.5</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>28</v>
       </c>
@@ -2222,14 +2253,14 @@
         <v>0.78125</v>
       </c>
       <c r="G48" s="1">
-        <f>F48-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H48">
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>29</v>
       </c>
@@ -2249,14 +2280,14 @@
         <v>0.78125</v>
       </c>
       <c r="G49" s="1">
-        <f>F49-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H49">
         <v>1.6</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>30</v>
       </c>
@@ -2276,14 +2307,14 @@
         <v>0.78125</v>
       </c>
       <c r="G50" s="1">
-        <f>F50-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H50">
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>31</v>
       </c>
@@ -2303,14 +2334,14 @@
         <v>0.78125</v>
       </c>
       <c r="G51" s="1">
-        <f>F51-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H51">
         <v>1.6</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>32</v>
       </c>
@@ -2330,14 +2361,14 @@
         <v>0.78125</v>
       </c>
       <c r="G52" s="1">
-        <f>F52-$G$1</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H52">
         <v>1.5</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>33</v>
       </c>
@@ -2357,14 +2388,14 @@
         <v>0.78125</v>
       </c>
       <c r="G53" s="1">
-        <f>F53-$G$1</f>
+        <f t="shared" ref="G53:G84" si="1">F53-$G$1</f>
         <v>0.25347222222222221</v>
       </c>
       <c r="H53">
         <v>1.5</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>34</v>
       </c>
@@ -2384,14 +2415,14 @@
         <v>0.78125</v>
       </c>
       <c r="G54" s="1">
-        <f>F54-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H54">
         <v>1.5</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>35</v>
       </c>
@@ -2411,14 +2442,14 @@
         <v>0.78125</v>
       </c>
       <c r="G55" s="1">
-        <f>F55-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H55">
         <v>1.6</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>36</v>
       </c>
@@ -2438,14 +2469,14 @@
         <v>0.78125</v>
       </c>
       <c r="G56" s="1">
-        <f>F56-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
       <c r="H56">
         <v>1.6</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>37</v>
       </c>
@@ -2465,11 +2496,11 @@
         <v>0.78125</v>
       </c>
       <c r="G57" s="1">
-        <f>F57-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>38</v>
       </c>
@@ -2489,11 +2520,11 @@
         <v>0.78125</v>
       </c>
       <c r="G58" s="1">
-        <f>F58-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>39</v>
       </c>
@@ -2513,11 +2544,11 @@
         <v>0.78125</v>
       </c>
       <c r="G59" s="1">
-        <f>F59-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>40</v>
       </c>
@@ -2537,11 +2568,11 @@
         <v>0.78125</v>
       </c>
       <c r="G60" s="1">
-        <f>F60-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>41</v>
       </c>
@@ -2561,11 +2592,11 @@
         <v>0.78125</v>
       </c>
       <c r="G61" s="1">
-        <f>F61-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>42</v>
       </c>
@@ -2585,11 +2616,11 @@
         <v>0.78125</v>
       </c>
       <c r="G62" s="1">
-        <f>F62-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>43</v>
       </c>
@@ -2609,11 +2640,11 @@
         <v>0.78125</v>
       </c>
       <c r="G63" s="1">
-        <f>F63-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>44</v>
       </c>
@@ -2633,11 +2664,11 @@
         <v>0.78125</v>
       </c>
       <c r="G64" s="1">
-        <f>F64-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>45</v>
       </c>
@@ -2657,11 +2688,11 @@
         <v>0.78125</v>
       </c>
       <c r="G65" s="1">
-        <f>F65-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>46</v>
       </c>
@@ -2681,11 +2712,11 @@
         <v>0.78125</v>
       </c>
       <c r="G66" s="1">
-        <f>F66-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>47</v>
       </c>
@@ -2705,11 +2736,11 @@
         <v>0.78125</v>
       </c>
       <c r="G67" s="1">
-        <f>F67-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>48</v>
       </c>
@@ -2729,11 +2760,11 @@
         <v>0.78125</v>
       </c>
       <c r="G68" s="1">
-        <f>F68-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.25347222222222221</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>49</v>
       </c>
@@ -2753,11 +2784,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G69" s="1">
-        <f>F69-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>50</v>
       </c>
@@ -2777,11 +2808,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G70" s="1">
-        <f>F70-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>51</v>
       </c>
@@ -2801,11 +2832,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G71" s="1">
-        <f>F71-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>52</v>
       </c>
@@ -2825,11 +2856,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G72" s="1">
-        <f>F72-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>53</v>
       </c>
@@ -2849,11 +2880,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G73" s="1">
-        <f>F73-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>54</v>
       </c>
@@ -2873,11 +2904,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G74" s="1">
-        <f>F74-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>55</v>
       </c>
@@ -2897,11 +2928,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G75" s="1">
-        <f>F75-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>56</v>
       </c>
@@ -2921,11 +2952,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G76" s="1">
-        <f>F76-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>57</v>
       </c>
@@ -2945,11 +2976,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G77" s="1">
-        <f>F77-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>58</v>
       </c>
@@ -2969,11 +3000,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G78" s="1">
-        <f>F78-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>59</v>
       </c>
@@ -2993,11 +3024,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G79" s="1">
-        <f>F79-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>60</v>
       </c>
@@ -3017,11 +3048,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G80" s="1">
-        <f>F80-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>61</v>
       </c>
@@ -3041,11 +3072,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G81" s="1">
-        <f>F81-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>62</v>
       </c>
@@ -3065,11 +3096,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G82" s="1">
-        <f>F82-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>63</v>
       </c>
@@ -3089,11 +3120,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G83" s="1">
-        <f>F83-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>64</v>
       </c>
@@ -3113,11 +3144,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G84" s="1">
-        <f>F84-$G$1</f>
+        <f t="shared" si="1"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>65</v>
       </c>
@@ -3137,11 +3168,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G85" s="1">
-        <f>F85-$G$1</f>
+        <f t="shared" ref="G85:G116" si="2">F85-$G$1</f>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>66</v>
       </c>
@@ -3161,11 +3192,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G86" s="1">
-        <f>F86-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>67</v>
       </c>
@@ -3185,11 +3216,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G87" s="1">
-        <f>F87-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>68</v>
       </c>
@@ -3209,11 +3240,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G88" s="1">
-        <f>F88-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>69</v>
       </c>
@@ -3233,11 +3264,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G89" s="1">
-        <f>F89-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>70</v>
       </c>
@@ -3257,11 +3288,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G90" s="1">
-        <f>F90-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>71</v>
       </c>
@@ -3281,11 +3312,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G91" s="1">
-        <f>F91-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>72</v>
       </c>
@@ -3305,11 +3336,11 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="G92" s="1">
-        <f>F92-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.21527777777777768</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>73</v>
       </c>
@@ -3329,11 +3360,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G93" s="1">
-        <f>F93-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>74</v>
       </c>
@@ -3353,11 +3384,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G94" s="1">
-        <f>F94-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>75</v>
       </c>
@@ -3377,11 +3408,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G95" s="1">
-        <f>F95-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>76</v>
       </c>
@@ -3401,11 +3432,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G96" s="1">
-        <f>F96-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>77</v>
       </c>
@@ -3425,11 +3456,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G97" s="1">
-        <f>F97-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>78</v>
       </c>
@@ -3449,11 +3480,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G98" s="1">
-        <f>F98-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>79</v>
       </c>
@@ -3473,11 +3504,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G99" s="1">
-        <f>F99-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>80</v>
       </c>
@@ -3497,11 +3528,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G100" s="1">
-        <f>F100-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>81</v>
       </c>
@@ -3521,11 +3552,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G101" s="1">
-        <f>F101-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>82</v>
       </c>
@@ -3545,11 +3576,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G102" s="1">
-        <f>F102-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>83</v>
       </c>
@@ -3569,11 +3600,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G103" s="1">
-        <f>F103-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>84</v>
       </c>
@@ -3593,11 +3624,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G104" s="1">
-        <f>F104-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>85</v>
       </c>
@@ -3617,11 +3648,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G105" s="1">
-        <f>F105-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>86</v>
       </c>
@@ -3641,11 +3672,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G106" s="1">
-        <f>F106-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>87</v>
       </c>
@@ -3665,11 +3696,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G107" s="1">
-        <f>F107-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>88</v>
       </c>
@@ -3689,11 +3720,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G108" s="1">
-        <f>F108-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>89</v>
       </c>
@@ -3713,11 +3744,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G109" s="1">
-        <f>F109-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>90</v>
       </c>
@@ -3737,11 +3768,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G110" s="1">
-        <f>F110-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>91</v>
       </c>
@@ -3761,11 +3792,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G111" s="1">
-        <f>F111-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>92</v>
       </c>
@@ -3785,11 +3816,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G112" s="1">
-        <f>F112-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>93</v>
       </c>
@@ -3809,11 +3840,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G113" s="1">
-        <f>F113-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>94</v>
       </c>
@@ -3833,11 +3864,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G114" s="1">
-        <f>F114-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>95</v>
       </c>
@@ -3857,11 +3888,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G115" s="1">
-        <f>F115-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>96</v>
       </c>
@@ -3881,14 +3912,14 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G116" s="1">
-        <f>F116-$G$1</f>
+        <f t="shared" si="2"/>
         <v>0.20138888888888884</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>97</v>
       </c>
@@ -3908,11 +3939,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G118" s="1">
-        <f>F118-$G$1</f>
+        <f t="shared" ref="G118:G149" si="3">F118-$G$1</f>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>98</v>
       </c>
@@ -3932,11 +3963,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G119" s="1">
-        <f>F119-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>99</v>
       </c>
@@ -3956,11 +3987,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G120" s="1">
-        <f>F120-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>100</v>
       </c>
@@ -3980,11 +4011,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G121" s="1">
-        <f>F121-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>101</v>
       </c>
@@ -4004,11 +4035,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G122" s="1">
-        <f>F122-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>102</v>
       </c>
@@ -4028,11 +4059,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G123" s="1">
-        <f>F123-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>103</v>
       </c>
@@ -4052,11 +4083,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G124" s="1">
-        <f>F124-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>104</v>
       </c>
@@ -4076,11 +4107,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G125" s="1">
-        <f>F125-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>105</v>
       </c>
@@ -4100,11 +4131,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G126" s="1">
-        <f>F126-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>106</v>
       </c>
@@ -4124,11 +4155,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G127" s="1">
-        <f>F127-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>107</v>
       </c>
@@ -4148,11 +4179,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G128" s="1">
-        <f>F128-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>108</v>
       </c>
@@ -4172,11 +4203,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G129" s="1">
-        <f>F129-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>109</v>
       </c>
@@ -4196,11 +4227,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G130" s="1">
-        <f>F130-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>110</v>
       </c>
@@ -4220,11 +4251,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G131" s="1">
-        <f>F131-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>111</v>
       </c>
@@ -4244,11 +4275,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G132" s="1">
-        <f>F132-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>112</v>
       </c>
@@ -4268,11 +4299,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G133" s="1">
-        <f>F133-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>113</v>
       </c>
@@ -4292,11 +4323,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G134" s="1">
-        <f>F134-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>114</v>
       </c>
@@ -4316,11 +4347,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G135" s="1">
-        <f>F135-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>115</v>
       </c>
@@ -4340,11 +4371,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G136" s="1">
-        <f>F136-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>116</v>
       </c>
@@ -4364,11 +4395,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G137" s="1">
-        <f>F137-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>117</v>
       </c>
@@ -4388,11 +4419,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G138" s="1">
-        <f>F138-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>118</v>
       </c>
@@ -4412,11 +4443,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G139" s="1">
-        <f>F139-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>119</v>
       </c>
@@ -4436,11 +4467,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G140" s="1">
-        <f>F140-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>120</v>
       </c>
@@ -4460,11 +4491,11 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="G141" s="1">
-        <f>F141-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.31944444444444442</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>121</v>
       </c>
@@ -4484,11 +4515,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G142" s="1">
-        <f>F142-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>122</v>
       </c>
@@ -4508,11 +4539,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G143" s="1">
-        <f>F143-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>123</v>
       </c>
@@ -4532,11 +4563,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G144" s="1">
-        <f>F144-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>124</v>
       </c>
@@ -4556,11 +4587,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G145" s="1">
-        <f>F145-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>125</v>
       </c>
@@ -4580,11 +4611,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G146" s="1">
-        <f>F146-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>126</v>
       </c>
@@ -4604,11 +4635,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G147" s="1">
-        <f>F147-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>127</v>
       </c>
@@ -4628,11 +4659,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G148" s="1">
-        <f>F148-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>128</v>
       </c>
@@ -4652,11 +4683,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G149" s="1">
-        <f>F149-$G$1</f>
+        <f t="shared" si="3"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>129</v>
       </c>
@@ -4676,11 +4707,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G150" s="1">
-        <f>F150-$G$1</f>
+        <f t="shared" ref="G150:G181" si="4">F150-$G$1</f>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>130</v>
       </c>
@@ -4700,11 +4731,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G151" s="1">
-        <f>F151-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>131</v>
       </c>
@@ -4724,11 +4755,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G152" s="1">
-        <f>F152-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>132</v>
       </c>
@@ -4748,11 +4779,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G153" s="1">
-        <f>F153-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>133</v>
       </c>
@@ -4772,11 +4803,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G154" s="1">
-        <f>F154-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>134</v>
       </c>
@@ -4796,11 +4827,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G155" s="1">
-        <f>F155-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>135</v>
       </c>
@@ -4820,11 +4851,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G156" s="1">
-        <f>F156-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>136</v>
       </c>
@@ -4844,11 +4875,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G157" s="1">
-        <f>F157-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>137</v>
       </c>
@@ -4868,11 +4899,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G158" s="1">
-        <f>F158-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>138</v>
       </c>
@@ -4892,11 +4923,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G159" s="1">
-        <f>F159-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>139</v>
       </c>
@@ -4916,11 +4947,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G160" s="1">
-        <f>F160-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>140</v>
       </c>
@@ -4940,11 +4971,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G161" s="1">
-        <f>F161-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>141</v>
       </c>
@@ -4964,11 +4995,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G162" s="1">
-        <f>F162-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>142</v>
       </c>
@@ -4988,11 +5019,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G163" s="1">
-        <f>F163-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>143</v>
       </c>
@@ -5012,11 +5043,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G164" s="1">
-        <f>F164-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>144</v>
       </c>
@@ -5036,11 +5067,11 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="G165" s="1">
-        <f>F165-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.29513888888888884</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>145</v>
       </c>
@@ -5060,11 +5091,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G166" s="1">
-        <f>F166-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>146</v>
       </c>
@@ -5084,11 +5115,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G167" s="1">
-        <f>F167-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>147</v>
       </c>
@@ -5108,11 +5139,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G168" s="1">
-        <f>F168-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>148</v>
       </c>
@@ -5132,11 +5163,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G169" s="1">
-        <f>F169-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>149</v>
       </c>
@@ -5156,11 +5187,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G170" s="1">
-        <f>F170-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>150</v>
       </c>
@@ -5180,11 +5211,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G171" s="1">
-        <f>F171-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>151</v>
       </c>
@@ -5204,11 +5235,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G172" s="1">
-        <f>F172-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>152</v>
       </c>
@@ -5228,11 +5259,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G173" s="1">
-        <f>F173-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>153</v>
       </c>
@@ -5252,11 +5283,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G174" s="1">
-        <f>F174-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>157</v>
       </c>
@@ -5276,11 +5307,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G175" s="1">
-        <f>F175-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>158</v>
       </c>
@@ -5300,11 +5331,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G176" s="1">
-        <f>F176-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>159</v>
       </c>
@@ -5324,11 +5355,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G177" s="1">
-        <f>F177-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>160</v>
       </c>
@@ -5348,11 +5379,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G178" s="1">
-        <f>F178-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>161</v>
       </c>
@@ -5372,11 +5403,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G179" s="1">
-        <f>F179-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>162</v>
       </c>
@@ -5396,11 +5427,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G180" s="1">
-        <f>F180-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>163</v>
       </c>
@@ -5420,11 +5451,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G181" s="1">
-        <f>F181-$G$1</f>
+        <f t="shared" si="4"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>164</v>
       </c>
@@ -5444,11 +5475,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G182" s="1">
-        <f>F182-$G$1</f>
+        <f t="shared" ref="G182:G213" si="5">F182-$G$1</f>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>165</v>
       </c>
@@ -5468,11 +5499,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G183" s="1">
-        <f>F183-$G$1</f>
+        <f t="shared" si="5"/>
         <v>0.27430555555555558</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>169</v>
       </c>
@@ -5492,11 +5523,14 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G184" s="1">
-        <f>F184-$G$1</f>
+        <f t="shared" si="5"/>
         <v>0.27430555555555558</v>
       </c>
-    </row>
-    <row r="185" spans="1:7">
+      <c r="I184" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>170</v>
       </c>
@@ -5516,11 +5550,14 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G185" s="1">
-        <f>F185-$G$1</f>
+        <f t="shared" si="5"/>
         <v>0.27430555555555558</v>
       </c>
-    </row>
-    <row r="186" spans="1:7">
+      <c r="I185" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>171</v>
       </c>
@@ -5540,11 +5577,14 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G186" s="1">
-        <f>F186-$G$1</f>
+        <f t="shared" si="5"/>
         <v>0.27430555555555558</v>
       </c>
-    </row>
-    <row r="187" spans="1:7">
+      <c r="I186" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>172</v>
       </c>
@@ -5564,8 +5604,11 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="G187" s="1">
-        <f>F187-$G$1</f>
+        <f t="shared" si="5"/>
         <v>0.27430555555555558</v>
+      </c>
+      <c r="I187" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -5580,14 +5623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
@@ -5596,7 +5639,7 @@
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="29" customHeight="1">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>38</v>
       </c>
@@ -5622,7 +5665,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0.54166666666666663</v>
       </c>
@@ -5648,7 +5691,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.54166666666666663</v>
       </c>
@@ -5674,7 +5717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.5625</v>
       </c>
@@ -5700,7 +5743,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.5625</v>
       </c>
@@ -5726,7 +5769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.5625</v>
       </c>
@@ -5752,7 +5795,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.57291666666666663</v>
       </c>
@@ -5778,7 +5821,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.57291666666666663</v>
       </c>
@@ -5804,7 +5847,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.57291666666666663</v>
       </c>
@@ -5830,7 +5873,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.57291666666666663</v>
       </c>
@@ -5856,7 +5899,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.57291666666666663</v>
       </c>
@@ -5882,7 +5925,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0.57291666666666663</v>
       </c>
@@ -5908,7 +5951,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.61458333333333337</v>
       </c>
@@ -5934,7 +5977,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0.61458333333333337</v>
       </c>
@@ -5960,7 +6003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0.61458333333333337</v>
       </c>
@@ -5986,7 +6029,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0.61458333333333337</v>
       </c>
@@ -6012,7 +6055,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0.61458333333333337</v>
       </c>
@@ -6038,7 +6081,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0.61458333333333337</v>
       </c>
@@ -6064,7 +6107,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0.65625</v>
       </c>
@@ -6090,7 +6133,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.65625</v>
       </c>
@@ -6116,7 +6159,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.65625</v>
       </c>
@@ -6142,7 +6185,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0.65625</v>
       </c>
@@ -6168,7 +6211,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0.69791666666666663</v>
       </c>
@@ -6194,7 +6237,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0.69791666666666663</v>
       </c>
@@ -6220,7 +6263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0.69791666666666663</v>
       </c>
@@ -6246,7 +6289,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0.69791666666666663</v>
       </c>

</xml_diff>